<commit_message>
sample num 7 is cleaned up
</commit_message>
<xml_diff>
--- a/Test-Data/Example7.xlsx
+++ b/Test-Data/Example7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AI-MRO\Data\Test-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilu\Navid\EA\EA-Heuristic\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6A342A-3140-4389-9BA9-B4D61E53FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1D722C-D268-4EBA-8F13-DA4858BA3A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
+    <workbookView xWindow="3160" yWindow="6450" windowWidth="32310" windowHeight="16590" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
   </bookViews>
   <sheets>
     <sheet name="Aircraft_scheduling" sheetId="1" r:id="rId1"/>
@@ -847,20 +847,20 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.08203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="3"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
@@ -883,7 +883,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -908,7 +908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>102</v>
@@ -934,7 +934,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>103</v>
@@ -949,8 +949,7 @@
         <v>45748</v>
       </c>
       <c r="E4" s="9">
-        <f>C4+0.93</f>
-        <v>1.2911111111111111</v>
+        <v>0.2911111111111111</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
@@ -960,7 +959,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -975,18 +974,17 @@
         <v>45748</v>
       </c>
       <c r="E5" s="9">
-        <f>C5+0.86</f>
-        <v>1.2488888888888889</v>
+        <v>0.24888888888888891</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>0.8600000000000001</v>
+        <v>0.86</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -1001,18 +999,17 @@
         <v>45748</v>
       </c>
       <c r="E6" s="9">
-        <f>C6+0.743</f>
-        <v>1.2117499999999999</v>
+        <v>0.21174768518518519</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="0"/>
-        <v>0.74299999999999988</v>
+        <v>0.74299768518518516</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -1037,7 +1034,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -1062,7 +1059,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -1077,18 +1074,17 @@
         <v>45748</v>
       </c>
       <c r="E9" s="9">
-        <f>C9+0.72</f>
-        <v>1.2790277777777779</v>
+        <v>0.27902777777777776</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="0"/>
-        <v>0.72000000000000008</v>
+        <v>0.72</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -1103,18 +1099,17 @@
         <v>45748</v>
       </c>
       <c r="E10" s="9">
-        <f>C10+0.59</f>
-        <v>1.1837499999999999</v>
+        <v>0.18375</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="0"/>
-        <v>0.58999999999999986</v>
+        <v>0.59</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -1129,18 +1124,17 @@
         <v>45749</v>
       </c>
       <c r="E11" s="9">
-        <f>C11+0.745</f>
-        <v>1.4429166666666666</v>
+        <v>0.44291666666666668</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="0"/>
-        <v>0.745</v>
+        <v>0.74500000000000011</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -1155,8 +1149,7 @@
         <v>45749</v>
       </c>
       <c r="E12" s="9">
-        <f>C12+0.63</f>
-        <v>1.3556944444444445</v>
+        <v>0.35569444444444448</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="0"/>
@@ -1166,7 +1159,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -1181,18 +1174,17 @@
         <v>45749</v>
       </c>
       <c r="E13" s="9">
-        <f>C13+0.81</f>
-        <v>1.5877777777777777</v>
+        <v>0.58777777777777784</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="0"/>
-        <v>0.80999999999999994</v>
+        <v>0.81</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -1207,18 +1199,17 @@
         <v>45749</v>
       </c>
       <c r="E14" s="9">
-        <f>C14+0.93</f>
-        <v>1.7320833333333334</v>
+        <v>0.73208333333333331</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="0"/>
-        <v>0.93</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -1233,18 +1224,17 @@
         <v>45749</v>
       </c>
       <c r="E15" s="9">
-        <f>C15+0.79</f>
-        <v>1.5990277777777777</v>
+        <v>0.59902777777777783</v>
       </c>
       <c r="F15" s="9">
         <f t="shared" si="0"/>
-        <v>0.78999999999999992</v>
+        <v>0.79</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -1259,8 +1249,7 @@
         <v>45749</v>
       </c>
       <c r="E16" s="9">
-        <f>C16+0.87</f>
-        <v>1.6963888888888889</v>
+        <v>0.69638888888888895</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" si="0"/>
@@ -1270,7 +1259,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -1285,18 +1274,17 @@
         <v>45749</v>
       </c>
       <c r="E17" s="9">
-        <f>C17+0.8</f>
-        <v>1.6472222222222221</v>
+        <v>0.64722222222222225</v>
       </c>
       <c r="F17" s="9">
         <f t="shared" si="0"/>
-        <v>0.79999999999999993</v>
+        <v>0.8</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1311,8 +1299,7 @@
         <v>45749</v>
       </c>
       <c r="E18" s="9">
-        <f>C18+0.91</f>
-        <v>1.7954166666666667</v>
+        <v>0.79541666666666666</v>
       </c>
       <c r="F18" s="9">
         <f t="shared" si="0"/>
@@ -1322,7 +1309,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -1347,7 +1334,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -1372,7 +1359,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -1397,131 +1384,131 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B53" s="8"/>
       <c r="D53" s="8"/>
     </row>
@@ -1538,18 +1525,18 @@
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="3"/>
-    <col min="4" max="4" width="10.875" style="4"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1566,7 +1553,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1590,7 +1577,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1614,7 +1601,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1638,7 +1625,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1662,7 +1649,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1686,7 +1673,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1710,7 +1697,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1734,7 +1721,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1758,7 +1745,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1782,7 +1769,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1806,7 +1793,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +1817,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1854,7 +1841,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1878,7 +1865,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1902,7 +1889,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1926,7 +1913,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1950,7 +1937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1974,7 +1961,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1998,7 +1985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2023,7 +2010,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2048,7 +2035,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2073,7 +2060,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2098,7 +2085,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2123,7 +2110,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2148,7 +2135,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
     </row>
   </sheetData>
@@ -2165,13 +2152,13 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>109</v>
       </c>
@@ -2179,7 +2166,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2190,7 +2177,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2201,7 +2188,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2212,7 +2199,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2223,7 +2210,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2234,7 +2221,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2245,7 +2232,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2256,7 +2243,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2267,7 +2254,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2278,7 +2265,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2289,7 +2276,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2300,7 +2287,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2311,7 +2298,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2322,7 +2309,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2333,7 +2320,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2344,7 +2331,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2355,7 +2342,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2366,7 +2353,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2377,7 +2364,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2388,7 +2375,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2399,7 +2386,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2410,7 +2397,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2421,7 +2408,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2432,7 +2419,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2443,7 +2430,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2454,7 +2441,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2465,7 +2452,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2476,7 +2463,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2487,7 +2474,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2498,7 +2485,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2509,7 +2496,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2520,7 +2507,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2531,7 +2518,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2542,7 +2529,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2553,7 +2540,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2564,7 +2551,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>

</xml_diff>